<commit_message>
completed project 4 Maven safety council
</commit_message>
<xml_diff>
--- a/Excel/Statistics for Data Analysis/StatisticsforDataAnalysis-221118-112009/Projects/Car_Speeds.xlsx
+++ b/Excel/Statistics for Data Analysis/StatisticsforDataAnalysis-221118-112009/Projects/Car_Speeds.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25904"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\Author Drive (E. Ruiz)\Excel Statistics\Course Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorgesoto/Desktop/Maven_Analytics/Excel/Statistics for Data Analysis/StatisticsforDataAnalysis-221118-112009/Projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF4125C-ECC3-4641-874E-AE1199D68704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1036FC7-84D2-ED49-AE60-35DB7DB7BDA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{0E4CE17A-2A24-46D2-A636-177A1F161D3F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="20140" xr2:uid="{0E4CE17A-2A24-46D2-A636-177A1F161D3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,19 +19,16 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$301</definedName>
     <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$1</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$2:$A$101</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$A$2:$A$101</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$B$2:$B$101</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$C$2:$C$101</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$C$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$C$2:$C$101</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$1</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$2:$B$101</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$1</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$C$2:$C$101</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!#REF!</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$A$1</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$A$2:$A$301</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$A$1</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$A$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$A$2:$A$101</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$B$2:$B$101</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Before</t>
   </si>
@@ -64,12 +61,116 @@
   <si>
     <t>After</t>
   </si>
+  <si>
+    <t>Sample Size (n):</t>
+  </si>
+  <si>
+    <t>n-1:</t>
+  </si>
+  <si>
+    <t>Mean (x̄):</t>
+  </si>
+  <si>
+    <r>
+      <t>Variance (s</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>):</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/n:</t>
+    </r>
+  </si>
+  <si>
+    <t>Ho:</t>
+  </si>
+  <si>
+    <t>Ha:</t>
+  </si>
+  <si>
+    <t>Alpha:</t>
+  </si>
+  <si>
+    <t>Standard Error:</t>
+  </si>
+  <si>
+    <t>Test Statistic (t):</t>
+  </si>
+  <si>
+    <t>Degrees of Freedom:</t>
+  </si>
+  <si>
+    <t>P-Value:</t>
+  </si>
+  <si>
+    <t>d &lt; 0</t>
+  </si>
+  <si>
+    <t>d &gt;= 0</t>
+  </si>
+  <si>
+    <t>REJECT!</t>
+  </si>
+  <si>
+    <t>FAIL to REJECT!</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="4">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.00000"/>
+    <numFmt numFmtId="169" formatCode="0.0000"/>
+    <numFmt numFmtId="174" formatCode="#,##0.000000"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,8 +186,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -99,8 +232,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -108,13 +247,78 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
+      <right style="thin">
+        <color theme="2"/>
+      </right>
+      <top style="thin">
+        <color theme="2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -132,8 +336,830 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.1</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.3</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="2">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.5</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{90788C2E-629F-A140-8733-B67767B21847}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.0</cx:f>
+              <cx:v>Before</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{899DA6BE-C3A3-9049-AAE7-9C0A7FD746A4}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:v>Shortly After</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{F8666DF9-C105-0E49-AB43-3E814B64987F}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:v>After</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="2"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="406">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Chart 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABD26049-5B61-CFB3-B712-8E1B52329DDE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2559050" y="2146300"/>
+              <a:ext cx="4572000" cy="4978400"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C620911-4A24-C58E-EF4E-B4EEBFCDC8FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7340600" y="2717800"/>
+          <a:ext cx="4737100" cy="1663700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>In</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" baseline="0"/>
+            <a:t> fact confirm with 90% confidence that there is a significant reduction in the average speeds </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>shortly after </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" baseline="0"/>
+            <a:t>putting up the sign.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" baseline="0"/>
+            <a:t>But we cant confirm with a 95% confidence that there is a significant reduction in the average speeds </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>after</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" baseline="0"/>
+            <a:t> putting up the signs.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -421,7 +1447,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -429,18 +1455,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFAA3F91-60B7-4425-BC47-0A35373AFB44}">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:V101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" customWidth="1"/>
+    <col min="13" max="13" width="15.1640625" customWidth="1"/>
+    <col min="14" max="14" width="14" customWidth="1"/>
+    <col min="15" max="15" width="14.33203125" customWidth="1"/>
+    <col min="16" max="16" width="6" customWidth="1"/>
+    <col min="21" max="21" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,7 +1491,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>33</v>
       </c>
@@ -461,8 +1501,12 @@
       <c r="C2">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>34</v>
       </c>
@@ -472,8 +1516,30 @@
       <c r="C3">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="5"/>
+      <c r="J3" s="16"/>
+      <c r="L3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>32</v>
       </c>
@@ -483,8 +1549,39 @@
       <c r="C4">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="3">
+        <f>COUNT(A2:A101)</f>
+        <v>100</v>
+      </c>
+      <c r="G4" s="3">
+        <f>COUNT(B2:B101)</f>
+        <v>100</v>
+      </c>
+      <c r="H4" s="3">
+        <f>COUNT(C2:C101)</f>
+        <v>100</v>
+      </c>
+      <c r="J4" s="7"/>
+      <c r="K4" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P4" s="9"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="12"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>32</v>
       </c>
@@ -494,8 +1591,38 @@
       <c r="C5">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="3">
+        <f>F4-1</f>
+        <v>99</v>
+      </c>
+      <c r="G5" s="3">
+        <f t="shared" ref="G5:H5" si="0">G4-1</f>
+        <v>99</v>
+      </c>
+      <c r="H5" s="3">
+        <f t="shared" si="0"/>
+        <v>99</v>
+      </c>
+      <c r="K5" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P5" s="9"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="13"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>26</v>
       </c>
@@ -505,8 +1632,37 @@
       <c r="C6">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="3">
+        <f>AVERAGE(A2:A101)</f>
+        <v>29.86</v>
+      </c>
+      <c r="G6" s="3">
+        <f t="shared" ref="G6:H6" si="1">AVERAGE(B2:B101)</f>
+        <v>27.75</v>
+      </c>
+      <c r="H6" s="3">
+        <f t="shared" si="1"/>
+        <v>29.81</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="14"/>
+    </row>
+    <row r="7" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>22</v>
       </c>
@@ -516,8 +1672,39 @@
       <c r="C7">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="3">
+        <f>VAR(A2:A101)</f>
+        <v>16.626666666666601</v>
+      </c>
+      <c r="G7" s="3">
+        <f t="shared" ref="G7:H7" si="2">VAR(B2:B101)</f>
+        <v>14.593434343434344</v>
+      </c>
+      <c r="H7" s="3">
+        <f t="shared" si="2"/>
+        <v>11.892828282828276</v>
+      </c>
+      <c r="K7" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="3">
+        <f>SQRT($F$8+G8)</f>
+        <v>0.56156438246881835</v>
+      </c>
+      <c r="M7" s="19">
+        <f>SQRT($F$8+H8)</f>
+        <v>0.5367268453883729</v>
+      </c>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="15"/>
+    </row>
+    <row r="8" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>31</v>
       </c>
@@ -527,8 +1714,34 @@
       <c r="C8">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="3">
+        <f>F7/F5</f>
+        <v>0.16794612794612729</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" ref="G8:H8" si="3">G7/G5</f>
+        <v>0.14740842771145801</v>
+      </c>
+      <c r="H8" s="3">
+        <f t="shared" si="3"/>
+        <v>0.12012957861442704</v>
+      </c>
+      <c r="K8" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" s="3">
+        <f>(G6-$F$6)/L7</f>
+        <v>-3.7573608046930578</v>
+      </c>
+      <c r="M8" s="3">
+        <f>(H6-$F$6)/M7</f>
+        <v>-9.3157255743041803E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>34</v>
       </c>
@@ -538,8 +1751,19 @@
       <c r="C9">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K9" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" s="3">
+        <f>($F$8+G8)^2/($F$8^2/$F$5+G8^2/G5)</f>
+        <v>197.16375701427577</v>
+      </c>
+      <c r="M9" s="3">
+        <f>($F$8+H8)^2/($F$8^2/$F$5+H8^2/H5)</f>
+        <v>192.69109638490266</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>31</v>
       </c>
@@ -549,8 +1773,19 @@
       <c r="C10">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="K10" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="3">
+        <f>_xlfn.T.DIST(L8,L9,TRUE)</f>
+        <v>1.1306437748771014E-4</v>
+      </c>
+      <c r="M10" s="3">
+        <f>_xlfn.T.DIST(M8,M9,TRUE)</f>
+        <v>0.46293788350479004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>32</v>
       </c>
@@ -561,7 +1796,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>37</v>
       </c>
@@ -571,8 +1806,14 @@
       <c r="C12">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="L12" t="s">
+        <v>17</v>
+      </c>
+      <c r="M12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>29</v>
       </c>
@@ -583,7 +1824,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>27</v>
       </c>
@@ -594,7 +1835,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>29</v>
       </c>
@@ -605,7 +1846,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>30</v>
       </c>
@@ -616,7 +1857,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>31</v>
       </c>
@@ -627,7 +1868,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>30</v>
       </c>
@@ -638,7 +1879,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>36</v>
       </c>
@@ -649,7 +1890,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>35</v>
       </c>
@@ -660,7 +1901,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>32</v>
       </c>
@@ -671,7 +1912,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>34</v>
       </c>
@@ -682,7 +1923,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>35</v>
       </c>
@@ -693,7 +1934,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>34</v>
       </c>
@@ -704,7 +1945,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>28</v>
       </c>
@@ -715,7 +1956,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>26</v>
       </c>
@@ -726,7 +1967,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>34</v>
       </c>
@@ -737,7 +1978,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>30</v>
       </c>
@@ -748,7 +1989,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>33</v>
       </c>
@@ -759,7 +2000,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>26</v>
       </c>
@@ -770,7 +2011,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>28</v>
       </c>
@@ -781,7 +2022,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>24</v>
       </c>
@@ -792,7 +2033,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>35</v>
       </c>
@@ -803,7 +2044,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>34</v>
       </c>
@@ -814,7 +2055,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -825,7 +2066,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>38</v>
       </c>
@@ -836,7 +2077,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>43</v>
       </c>
@@ -847,7 +2088,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>27</v>
       </c>
@@ -858,7 +2099,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>27</v>
       </c>
@@ -869,7 +2110,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>26</v>
       </c>
@@ -880,7 +2121,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>28</v>
       </c>
@@ -891,7 +2132,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>24</v>
       </c>
@@ -902,7 +2143,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>33</v>
       </c>
@@ -913,7 +2154,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>24</v>
       </c>
@@ -924,7 +2165,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>34</v>
       </c>
@@ -935,7 +2176,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>27</v>
       </c>
@@ -946,7 +2187,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>31</v>
       </c>
@@ -957,7 +2198,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>26</v>
       </c>
@@ -968,7 +2209,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>22</v>
       </c>
@@ -979,7 +2220,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>29</v>
       </c>
@@ -990,7 +2231,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>31</v>
       </c>
@@ -1001,7 +2242,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>29</v>
       </c>
@@ -1012,7 +2253,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>30</v>
       </c>
@@ -1023,7 +2264,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>35</v>
       </c>
@@ -1034,7 +2275,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>29</v>
       </c>
@@ -1045,7 +2286,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>30</v>
       </c>
@@ -1056,7 +2297,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>24</v>
       </c>
@@ -1067,7 +2308,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>36</v>
       </c>
@@ -1078,7 +2319,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>28</v>
       </c>
@@ -1089,7 +2330,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>36</v>
       </c>
@@ -1100,7 +2341,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>30</v>
       </c>
@@ -1111,7 +2352,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>28</v>
       </c>
@@ -1122,7 +2363,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>31</v>
       </c>
@@ -1133,7 +2374,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>28</v>
       </c>
@@ -1144,7 +2385,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>22</v>
       </c>
@@ -1155,7 +2396,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>38</v>
       </c>
@@ -1166,7 +2407,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>26</v>
       </c>
@@ -1177,7 +2418,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>28</v>
       </c>
@@ -1188,7 +2429,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>29</v>
       </c>
@@ -1199,7 +2440,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>27</v>
       </c>
@@ -1210,7 +2451,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>29</v>
       </c>
@@ -1221,7 +2462,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>25</v>
       </c>
@@ -1232,7 +2473,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>37</v>
       </c>
@@ -1243,7 +2484,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>36</v>
       </c>
@@ -1254,7 +2495,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>25</v>
       </c>
@@ -1265,7 +2506,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>32</v>
       </c>
@@ -1276,7 +2517,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>24</v>
       </c>
@@ -1287,7 +2528,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>26</v>
       </c>
@@ -1298,7 +2539,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>27</v>
       </c>
@@ -1309,7 +2550,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>29</v>
       </c>
@@ -1320,7 +2561,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>28</v>
       </c>
@@ -1331,7 +2572,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>26</v>
       </c>
@@ -1342,7 +2583,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>28</v>
       </c>
@@ -1353,7 +2594,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>26</v>
       </c>
@@ -1364,7 +2605,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>26</v>
       </c>
@@ -1375,7 +2616,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>28</v>
       </c>
@@ -1386,7 +2627,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>26</v>
       </c>
@@ -1397,7 +2638,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>28</v>
       </c>
@@ -1408,7 +2649,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>32</v>
       </c>
@@ -1419,7 +2660,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>35</v>
       </c>
@@ -1430,7 +2671,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>24</v>
       </c>
@@ -1441,7 +2682,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>30</v>
       </c>
@@ -1452,7 +2693,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>27</v>
       </c>
@@ -1463,7 +2704,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>30</v>
       </c>
@@ -1474,7 +2715,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>33</v>
       </c>
@@ -1485,7 +2726,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>31</v>
       </c>
@@ -1496,7 +2737,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>31</v>
       </c>
@@ -1507,7 +2748,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>28</v>
       </c>
@@ -1518,7 +2759,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>25</v>
       </c>
@@ -1529,7 +2770,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>29</v>
       </c>
@@ -1540,7 +2781,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>33</v>
       </c>
@@ -1552,6 +2793,12 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="U3:V3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>